<commit_message>
Making more reproducible and adding params direct for user. Fixed loops
</commit_message>
<xml_diff>
--- a/Project_Datasets/POIS.xlsx
+++ b/Project_Datasets/POIS.xlsx
@@ -19,57 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>ACADL</t>
+    <t>AACS</t>
   </si>
   <si>
-    <t>COX11</t>
+    <t>AADAT</t>
   </si>
   <si>
-    <t>FDX1L</t>
-  </si>
-  <si>
-    <t>FDXR</t>
-  </si>
-  <si>
-    <t>HEXA</t>
-  </si>
-  <si>
-    <t>IDI1</t>
-  </si>
-  <si>
-    <t>ISCU</t>
-  </si>
-  <si>
-    <t>NFS1</t>
-  </si>
-  <si>
-    <t>NRF1</t>
-  </si>
-  <si>
-    <t>PIGQ</t>
-  </si>
-  <si>
-    <t>PRDX1</t>
-  </si>
-  <si>
-    <t>SCLY</t>
-  </si>
-  <si>
-    <t>SLC25A25</t>
-  </si>
-  <si>
-    <t>SLC41A1</t>
-  </si>
-  <si>
-    <t>TXNRD1</t>
-  </si>
-  <si>
-    <t>TXNRD2</t>
-  </si>
-  <si>
-    <t>XYLT2</t>
+    <t>AAK1</t>
   </si>
 </sst>
 </file>
@@ -85,21 +43,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -107,61 +59,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,97 +345,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A17"/>
+      <selection activeCell="A4" sqref="A4:A4647"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding 1st tutorial video and longer POI list
</commit_message>
<xml_diff>
--- a/Project_Datasets/POIS.xlsx
+++ b/Project_Datasets/POIS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>AACS</t>
   </si>
@@ -28,15 +28,47 @@
   </si>
   <si>
     <t>AAK1</t>
+  </si>
+  <si>
+    <t>SPCS_HUMAN</t>
+  </si>
+  <si>
+    <t>SEPP1_HUMAN</t>
+  </si>
+  <si>
+    <t>ISCU_HUMAN</t>
+  </si>
+  <si>
+    <t>Q92911</t>
+  </si>
+  <si>
+    <t>P52789</t>
+  </si>
+  <si>
+    <t>Q9UPP1</t>
+  </si>
+  <si>
+    <t>O43772</t>
+  </si>
+  <si>
+    <t>P21796</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -63,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A4647"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,6 +401,46 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Including NAMPT in POI
</commit_message>
<xml_diff>
--- a/Project_Datasets/POIS.xlsx
+++ b/Project_Datasets/POIS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>AACS</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>P21796</t>
+  </si>
+  <si>
+    <t>NAMPT</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,6 +444,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>